<commit_message>
DB changes are done (pretty much). Now to change affected BOLs, followed by UI.
</commit_message>
<xml_diff>
--- a/Design to fully implement comics.xlsx
+++ b/Design to fully implement comics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Derive from one of the base five to begin a product or class. It may or may not keep the one original comic, but the instructor or designer will certainly add more comics while building up the product or class. The project will have a pricebump.</t>
   </si>
@@ -172,6 +172,36 @@
   </si>
   <si>
     <t>Recognized by</t>
+  </si>
+  <si>
+    <t>projects.isCoreProject = 1</t>
+  </si>
+  <si>
+    <t>projects.isClass = 1</t>
+  </si>
+  <si>
+    <t>projects.isProduct = 1</t>
+  </si>
+  <si>
+    <t>The three fields below are all = 0.</t>
+  </si>
+  <si>
+    <t>Changes to routeRetrieveProject</t>
+  </si>
+  <si>
+    <t>Changes to routeSaveProject</t>
+  </si>
+  <si>
+    <t>Changes to UntilityBO#routeSearchProjects</t>
+  </si>
+  <si>
+    <t>Types point to their project and to their comic. If they are part of a normal project, they point to the comic(s) for their project's origProjectId--this is the project that "owns" the comics.</t>
+  </si>
+  <si>
+    <t>Any project that isCoreProject, isClass or isProduct should be updated when being saved in order to retain its id.</t>
+  </si>
+  <si>
+    <t>These are also the only projects whose comics and comiccode need to be saved. Comics will be deleted and re-inserted. THAT'S NOT GOOD. Comic ids change. WHAT TO DO?</t>
   </si>
 </sst>
 </file>
@@ -273,6 +303,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1282700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9537700" y="317500"/>
+          <a:ext cx="6902450" cy="5016500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,6 +660,9 @@
       <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -578,6 +671,9 @@
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -586,6 +682,9 @@
       <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -594,6 +693,9 @@
       <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -645,149 +747,247 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="5"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="5"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="5"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Well into second half of new project dialog changes for creating classes and products.
</commit_message>
<xml_diff>
--- a/Design to fully implement comics.xlsx
+++ b/Design to fully implement comics.xlsx
@@ -120,9 +120,6 @@
     <t>Menu choice</t>
   </si>
   <si>
-    <t>We run a search for user-owned projects coming in and display their images. No one owns the 5 core projects, but a privileged user does own classes and products.</t>
-  </si>
-  <si>
     <t>Normal new project (will SaveAs; can view/run/interact with the comic but not edit it)</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
 o Classes
 o Products
 o All projects</t>
+  </si>
+  <si>
+    <t>We run a search for user-owned projects coming in and display their images. No one owns the 5 core projects, but a privileged user does own classes and products. Also, a privileged user can open a core project for editing types, system types or comic.</t>
   </si>
 </sst>
 </file>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,7 +648,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2"/>
     </row>
@@ -660,7 +660,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -671,7 +671,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -682,7 +682,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -693,7 +693,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -718,10 +718,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
@@ -729,18 +729,18 @@
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -748,32 +748,32 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -781,7 +781,7 @@
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -789,7 +789,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -809,7 +809,7 @@
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -832,7 +832,7 @@
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -854,19 +854,19 @@
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B43" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Minor changes. No affect.
</commit_message>
<xml_diff>
--- a/Design to fully implement comics.xlsx
+++ b/Design to fully implement comics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Derive from one of the base five to begin a product or class. It may or may not keep the one original comic, but the instructor or designer will certainly add more comics while building up the product or class. The project will have a pricebump.</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>We run a search for user-owned projects coming in and display their images. No one owns the 5 core projects, but a privileged user does own classes and products. Also, a privileged user can open a core project for editing types, system types or comic.</t>
+  </si>
+  <si>
+    <t>New project</t>
+  </si>
+  <si>
+    <t>Always saved as new. Name cannot conflict with another of user's projects.</t>
   </si>
 </sst>
 </file>
@@ -627,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,6 +990,14 @@
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
+    <row r="71" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Did some necessary cleaning up of new Product and new Class stuff.
</commit_message>
<xml_diff>
--- a/Design to fully implement comics.xlsx
+++ b/Design to fully implement comics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Derive from one of the base five to begin a product or class. It may or may not keep the one original comic, but the instructor or designer will certainly add more comics while building up the product or class. The project will have a pricebump.</t>
   </si>
@@ -203,10 +203,50 @@
     <t>We run a search for user-owned projects coming in and display their images. No one owns the 5 core projects, but a privileged user does own classes and products. Also, a privileged user can open a core project for editing types, system types or comic.</t>
   </si>
   <si>
-    <t>New project</t>
-  </si>
-  <si>
     <t>Always saved as new. Name cannot conflict with another of user's projects.</t>
+  </si>
+  <si>
+    <t>The project</t>
+  </si>
+  <si>
+    <t>The comics</t>
+  </si>
+  <si>
+    <t>System types</t>
+  </si>
+  <si>
+    <t>New project - user began by choosing one of the Core projects.</t>
+  </si>
+  <si>
+    <t>Search for/Open project - non-privileged user</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Save will always be Save as</t>
+  </si>
+  <si>
+    <t>If permitted, may work on comics</t>
+  </si>
+  <si>
+    <t>If permitted, may work on System types</t>
+  </si>
+  <si>
+    <t>Editing not permitted.</t>
+  </si>
+  <si>
+    <t>--If open own project, Save will replace former version by doing delete and re-insert--if name remains the same. If name has been changed, a new project will be created (if name is available).
+--If another's public project (not product or class) was opened, will do Save as (if name is available).
+--Will have to pay for Product or Class; save will always be Save as (if name is available)
+--Any project that is saved, now belongs to this user and isCoreProject, isClass and isProduct are all set = 0.</t>
+  </si>
+  <si>
+    <t>Search tags are always taken into consideration:
+o My own projects
+o All public projects
+o Products
+o Classes in next 3 months near zipcode ____</t>
   </si>
 </sst>
 </file>
@@ -250,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -264,7 +304,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,14 +365,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>349250</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>598055</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>1282700</xdr:rowOff>
     </xdr:to>
@@ -633,372 +684,451 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="36.81640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="21.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" style="4" customWidth="1"/>
+    <col min="3" max="5" width="36.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="34.26953125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="3" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="3" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C22" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="29" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="2"/>
+      <c r="B41" s="2"/>
       <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="3" t="s">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C42" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="3" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C43" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="50" spans="1:3" ht="261" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="3"/>
+      <c r="B51" s="5"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
-      <c r="B52" s="3"/>
+      <c r="B52" s="5"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
-      <c r="B53" s="3"/>
+      <c r="B53" s="5"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
-      <c r="B54" s="3"/>
+      <c r="B54" s="5"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="5"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:3" ht="319" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="3"/>
+      <c r="B56" s="5"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:3" ht="261" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="3"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="3"/>
+      <c r="B58" s="5"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="3"/>
+      <c r="B59" s="5"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="3"/>
+      <c r="B60" s="5"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B61" s="3"/>
+      <c r="B61" s="5"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="5"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="3"/>
+      <c r="B63" s="5"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="71" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C70" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>53</v>
+      <c r="D71" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="6"/>
+      <c r="B72" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" s="7"/>
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="1:6" ht="203" x14ac:dyDescent="0.35">
+      <c r="A74" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="6"/>
+      <c r="B75" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="C71:C72"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Reworked login page. Spiffed up Search for/Open Project dlg.
</commit_message>
<xml_diff>
--- a/Design to fully implement comics.xlsx
+++ b/Design to fully implement comics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Derive from one of the base five to begin a product or class. It may or may not keep the one original comic, but the instructor or designer will certainly add more comics while building up the product or class. The project will have a pricebump.</t>
   </si>
@@ -242,11 +242,54 @@
 --Any project that is saved, now belongs to this user and isCoreProject, isClass and isProduct are all set = 0.</t>
   </si>
   <si>
-    <t>Search tags are always taken into consideration:
-o My own projects
-o All public projects
-o Products
-o Classes in next 3 months near zipcode ____</t>
+    <t>Search tags (which are optional) are taken into consideration if entered.
+o Search only projects that I created
+o Search others' projects
+o Search for Products
+o Search for Classes near zipcode ____
+Notes:
+--others' projects must be public
+--products and classes must be active
+--classes must start within 3 months
+--will NEVER retrieve core projects
+--when searching for a specific person's projects, user can enter that person's userName (email) as a search tag</t>
+  </si>
+  <si>
+    <t>Search tags (which are optional) are taken into consideration if entered.
+o Retrieve Core projects
+o Search only projects that I created
+o Search others' projects
+o Search for Products
+o Search for Classes near zipcode ____
+Notes:
+--retrieving core projects will ignore tags
+--others' projects may be public or not
+--products and classes may be active or not
+--classes may start anytime--even in the past
+--zipcode is optional when searching for classes
+--will NEVER retrieve core projects
+--when searching for a specific person's projects, user can enter that person's userName (email) as a search tag</t>
+  </si>
+  <si>
+    <t>Retrieve core projects</t>
+  </si>
+  <si>
+    <t>Search only projects that I created</t>
+  </si>
+  <si>
+    <t>Search others' products</t>
+  </si>
+  <si>
+    <t>Search for Products</t>
+  </si>
+  <si>
+    <t>Search for Classes</t>
+  </si>
+  <si>
+    <t>Can save which will retain project id</t>
+  </si>
+  <si>
+    <t>Can work on comic if authorized, changing but not adding; can work on System Types if authorized.</t>
   </si>
 </sst>
 </file>
@@ -310,11 +353,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1058,13 +1101,13 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D71" s="4" t="s">
@@ -1078,11 +1121,11 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="6"/>
+      <c r="A72" s="8"/>
       <c r="B72" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="6"/>
+      <c r="C72" s="8"/>
       <c r="D72" s="4" t="s">
         <v>60</v>
       </c>
@@ -1094,11 +1137,11 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="7"/>
-      <c r="C73" s="7"/>
-    </row>
-    <row r="74" spans="1:6" ht="203" x14ac:dyDescent="0.35">
-      <c r="A74" s="6" t="s">
+      <c r="A73" s="6"/>
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -1113,14 +1156,48 @@
       <c r="E74" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="6"/>
+    <row r="75" spans="1:6" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="8"/>
       <c r="B75" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C76" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C77" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C78" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C79" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C80" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>